<commit_message>
CommonUtil, Screw Improve, StepControl, TipText
</commit_message>
<xml_diff>
--- a/Assets/Data/TextConfig.xlsx
+++ b/Assets/Data/TextConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProjects\FinalProject\Assets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7DEF6F-74F7-440E-9A94-E27830055781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A9F68E-DDD6-431D-B6A6-B8462B50D506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4215" yWindow="3195" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>key</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -48,6 +48,34 @@
   </si>
   <si>
     <t>English</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在放油螺栓处放置大号19号套筒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用大号棘轮扳手拆卸放油螺栓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>恭喜你完成训练</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Success0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -373,13 +401,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="29.875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -401,6 +432,39 @@
       </c>
       <c r="C2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10100</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>10101</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Screw Improve & First Complete Chapter
1. 第一章节步骤完成
2. 优化了拧螺丝几个bug
</commit_message>
<xml_diff>
--- a/Assets/Data/TextConfig.xlsx
+++ b/Assets/Data/TextConfig.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10545\Desktop\FinalProject\Assets\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProjects\FinalProject\Assets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AD83CB-F8E7-49F3-9391-69BAF8E81585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96C37C6-322E-49DB-9F56-4D9DFAE55AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5670" yWindow="1950" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29475" yWindow="-3090" windowWidth="12150" windowHeight="20835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
   <si>
     <t>key</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -298,6 +296,13 @@
   </si>
   <si>
     <t>模块</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在机油滤清器处放置EN-726-A机油滤清器扳手</t>
+  </si>
+  <si>
+    <t>使用大号棘轮扳手拆卸机油滤清器</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -623,15 +628,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="29.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -679,640 +684,662 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
+      <c r="A5">
+        <v>10103</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>63</v>
+        <v>73</v>
+      </c>
+      <c r="C5">
+        <v>10103</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>101</v>
+        <v>10104</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="C6">
-        <v>10100</v>
+        <v>10104</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>102</v>
+      <c r="A7" t="s">
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <v>10200</v>
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>10300</v>
+        <v>10100</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9">
-        <v>10400</v>
+        <v>10200</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10">
-        <v>10500</v>
+        <v>10300</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11">
-        <v>10600</v>
+        <v>10400</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12">
-        <v>10700</v>
+        <v>10500</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C13">
-        <v>10800</v>
+        <v>10600</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14">
-        <v>10900</v>
+        <v>10700</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15">
-        <v>11000</v>
+        <v>10800</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>201</v>
+        <v>109</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C16">
-        <v>20100</v>
+        <v>10900</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>202</v>
+        <v>110</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C17">
-        <v>20200</v>
+        <v>11000</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C18">
-        <v>20300</v>
+        <v>20100</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C19">
-        <v>20400</v>
+        <v>20200</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C20">
-        <v>20500</v>
+        <v>20300</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C21">
-        <v>20600</v>
+        <v>20400</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>301</v>
+        <v>205</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C22">
-        <v>30100</v>
+        <v>20500</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>302</v>
+        <v>206</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C23">
-        <v>30200</v>
+        <v>20600</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C24">
-        <v>30300</v>
+        <v>30100</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C25">
-        <v>30400</v>
+        <v>30200</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>401</v>
+        <v>303</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C26">
-        <v>40100</v>
+        <v>30300</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>501</v>
+        <v>304</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C27">
-        <v>50100</v>
+        <v>30400</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>502</v>
+        <v>401</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C28">
-        <v>50200</v>
+        <v>40100</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C29">
-        <v>50300</v>
+        <v>50100</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C30">
-        <v>50400</v>
+        <v>50200</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>601</v>
+        <v>503</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C31">
-        <v>60100</v>
+        <v>50300</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>602</v>
+        <v>504</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C32">
-        <v>60200</v>
+        <v>50400</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>1101</v>
+        <v>601</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C33">
-        <v>110100</v>
+        <v>60100</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>1102</v>
+        <v>602</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C34">
-        <v>110200</v>
+        <v>60200</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C35">
-        <v>110300</v>
+        <v>110100</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C36">
-        <v>110400</v>
+        <v>110200</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C37">
-        <v>110500</v>
+        <v>110300</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C38">
-        <v>110600</v>
+        <v>110400</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C39">
-        <v>110700</v>
+        <v>110500</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C40">
-        <v>110800</v>
+        <v>110600</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C41">
-        <v>110900</v>
+        <v>110700</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="B42" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C42">
-        <v>111000</v>
+        <v>110800</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>1201</v>
+        <v>1109</v>
       </c>
       <c r="B43" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C43">
-        <v>120100</v>
+        <v>110900</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>1202</v>
+        <v>1110</v>
       </c>
       <c r="B44" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="C44">
-        <v>120200</v>
+        <v>111000</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C45">
-        <v>120300</v>
+        <v>120100</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="C46">
-        <v>120400</v>
+        <v>120200</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C47">
-        <v>120500</v>
+        <v>120300</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C48">
-        <v>120600</v>
+        <v>120400</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>1301</v>
+        <v>1205</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C49">
-        <v>130100</v>
+        <v>120500</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>1302</v>
+        <v>1206</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C50">
-        <v>130200</v>
+        <v>120600</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C51">
-        <v>130300</v>
+        <v>130100</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C52">
-        <v>130400</v>
+        <v>130200</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>1401</v>
+        <v>1303</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C53">
-        <v>140100</v>
+        <v>130300</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>1501</v>
+        <v>1304</v>
       </c>
       <c r="B54" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C54">
-        <v>150100</v>
+        <v>130400</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>1502</v>
+        <v>1401</v>
       </c>
       <c r="B55" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C55">
-        <v>150200</v>
+        <v>140100</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>1503</v>
+        <v>1501</v>
       </c>
       <c r="B56" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C56">
-        <v>150300</v>
+        <v>150100</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="B57" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C57">
-        <v>150400</v>
+        <v>150200</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>1601</v>
+        <v>1503</v>
       </c>
       <c r="B58" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C58">
-        <v>160100</v>
+        <v>150300</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
+        <v>1504</v>
+      </c>
+      <c r="B59" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59">
+        <v>150400</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>1601</v>
+      </c>
+      <c r="B60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60">
+        <v>160100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61">
         <v>1602</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B61" t="s">
         <v>62</v>
       </c>
-      <c r="C59">
+      <c r="C61">
         <v>160200</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>64</v>
-      </c>
-      <c r="B60" t="s">
-        <v>70</v>
-      </c>
-      <c r="C60" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>65</v>
-      </c>
-      <c r="B61" t="s">
-        <v>71</v>
-      </c>
-      <c r="C61" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63" t="s">
+        <v>71</v>
+      </c>
+      <c r="C63" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>66</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B64" t="s">
         <v>72</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C64" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>